<commit_message>
count of people over time in some canteen
</commit_message>
<xml_diff>
--- a/gen/spend_amount_per_perchase_lunch_dinner_graph.xlsx
+++ b/gen/spend_amount_per_perchase_lunch_dinner_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8805" tabRatio="571" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="spend_amount_per_perchase_lunch" sheetId="1" r:id="rId1"/>
@@ -1090,11 +1090,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375905032"/>
-        <c:axId val="375201088"/>
+        <c:axId val="416143160"/>
+        <c:axId val="435306272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375905032"/>
+        <c:axId val="416143160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1136,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375201088"/>
+        <c:crossAx val="435306272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1144,7 +1144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375201088"/>
+        <c:axId val="435306272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375905032"/>
+        <c:crossAx val="416143160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1444,11 +1444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375625400"/>
-        <c:axId val="375630496"/>
+        <c:axId val="435293024"/>
+        <c:axId val="435293416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375625400"/>
+        <c:axId val="435293024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1490,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375630496"/>
+        <c:crossAx val="435293416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1498,7 +1498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375630496"/>
+        <c:axId val="435293416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1549,7 +1549,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375625400"/>
+        <c:crossAx val="435293024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1798,11 +1798,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376373008"/>
-        <c:axId val="376373400"/>
+        <c:axId val="435310976"/>
+        <c:axId val="435294200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376373008"/>
+        <c:axId val="435310976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1844,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376373400"/>
+        <c:crossAx val="435294200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1852,7 +1852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376373400"/>
+        <c:axId val="435294200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1903,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376373008"/>
+        <c:crossAx val="435310976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2152,11 +2152,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376374184"/>
-        <c:axId val="376374576"/>
+        <c:axId val="435294984"/>
+        <c:axId val="435295376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376374184"/>
+        <c:axId val="435294984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2198,7 +2198,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376374576"/>
+        <c:crossAx val="435295376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2206,7 +2206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376374576"/>
+        <c:axId val="435295376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2257,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376374184"/>
+        <c:crossAx val="435294984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2506,11 +2506,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376375360"/>
-        <c:axId val="376375752"/>
+        <c:axId val="435296160"/>
+        <c:axId val="435296552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376375360"/>
+        <c:axId val="435296160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,7 +2552,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376375752"/>
+        <c:crossAx val="435296552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2560,7 +2560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376375752"/>
+        <c:axId val="435296552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2611,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376375360"/>
+        <c:crossAx val="435296160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2860,11 +2860,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376376536"/>
-        <c:axId val="376376928"/>
+        <c:axId val="435297336"/>
+        <c:axId val="422137792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376376536"/>
+        <c:axId val="435297336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2906,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376376928"/>
+        <c:crossAx val="422137792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376376928"/>
+        <c:axId val="422137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2965,7 +2965,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376376536"/>
+        <c:crossAx val="435297336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3214,11 +3214,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376377712"/>
-        <c:axId val="376378104"/>
+        <c:axId val="422138576"/>
+        <c:axId val="422138968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376377712"/>
+        <c:axId val="422138576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3260,7 +3260,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376378104"/>
+        <c:crossAx val="422138968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3268,7 +3268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376378104"/>
+        <c:axId val="422138968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3319,7 +3319,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376377712"/>
+        <c:crossAx val="422138576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3568,11 +3568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376378888"/>
-        <c:axId val="376379280"/>
+        <c:axId val="422139752"/>
+        <c:axId val="422140144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376378888"/>
+        <c:axId val="422139752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3614,7 +3614,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376379280"/>
+        <c:crossAx val="422140144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3622,7 +3622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376379280"/>
+        <c:axId val="422140144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3673,7 +3673,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376378888"/>
+        <c:crossAx val="422139752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3922,11 +3922,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376380064"/>
-        <c:axId val="376380456"/>
+        <c:axId val="422140928"/>
+        <c:axId val="422141320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376380064"/>
+        <c:axId val="422140928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3968,7 +3968,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376380456"/>
+        <c:crossAx val="422141320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3976,7 +3976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376380456"/>
+        <c:axId val="422141320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4027,7 +4027,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376380064"/>
+        <c:crossAx val="422140928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4276,11 +4276,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376477072"/>
-        <c:axId val="376477464"/>
+        <c:axId val="422142104"/>
+        <c:axId val="422142496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376477072"/>
+        <c:axId val="422142104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4322,7 +4322,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376477464"/>
+        <c:crossAx val="422142496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4330,7 +4330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376477464"/>
+        <c:axId val="422142496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4381,7 +4381,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376477072"/>
+        <c:crossAx val="422142104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4630,11 +4630,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376478248"/>
-        <c:axId val="376478640"/>
+        <c:axId val="422143280"/>
+        <c:axId val="422143672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376478248"/>
+        <c:axId val="422143280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4676,7 +4676,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376478640"/>
+        <c:crossAx val="422143672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4684,7 +4684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376478640"/>
+        <c:axId val="422143672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4735,7 +4735,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376478248"/>
+        <c:crossAx val="422143280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4984,11 +4984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375264672"/>
-        <c:axId val="375265056"/>
+        <c:axId val="435307448"/>
+        <c:axId val="435307840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375264672"/>
+        <c:axId val="435307448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5030,7 +5030,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375265056"/>
+        <c:crossAx val="435307840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5038,7 +5038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375265056"/>
+        <c:axId val="435307840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5089,7 +5089,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375264672"/>
+        <c:crossAx val="435307448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5338,11 +5338,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376479816"/>
-        <c:axId val="376480208"/>
+        <c:axId val="422144848"/>
+        <c:axId val="422145240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376479816"/>
+        <c:axId val="422144848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5384,7 +5384,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376480208"/>
+        <c:crossAx val="422145240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5392,7 +5392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376480208"/>
+        <c:axId val="422145240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5443,7 +5443,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376479816"/>
+        <c:crossAx val="422144848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5692,11 +5692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376480600"/>
-        <c:axId val="376480992"/>
+        <c:axId val="419618744"/>
+        <c:axId val="419619136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376480600"/>
+        <c:axId val="419618744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5738,7 +5738,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376480992"/>
+        <c:crossAx val="419619136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5746,7 +5746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376480992"/>
+        <c:axId val="419619136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5797,7 +5797,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376480600"/>
+        <c:crossAx val="419618744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6046,11 +6046,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376481776"/>
-        <c:axId val="376482168"/>
+        <c:axId val="419619920"/>
+        <c:axId val="419620312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376481776"/>
+        <c:axId val="419619920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6092,7 +6092,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376482168"/>
+        <c:crossAx val="419620312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6100,7 +6100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376482168"/>
+        <c:axId val="419620312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6151,7 +6151,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376481776"/>
+        <c:crossAx val="419619920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6400,11 +6400,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376482952"/>
-        <c:axId val="376483344"/>
+        <c:axId val="419621096"/>
+        <c:axId val="419621488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376482952"/>
+        <c:axId val="419621096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6446,7 +6446,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376483344"/>
+        <c:crossAx val="419621488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6454,7 +6454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376483344"/>
+        <c:axId val="419621488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6505,7 +6505,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376482952"/>
+        <c:crossAx val="419621096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6754,11 +6754,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376484128"/>
-        <c:axId val="376715264"/>
+        <c:axId val="419622272"/>
+        <c:axId val="419622664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376484128"/>
+        <c:axId val="419622272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6800,7 +6800,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376715264"/>
+        <c:crossAx val="419622664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6808,7 +6808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376715264"/>
+        <c:axId val="419622664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6859,7 +6859,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376484128"/>
+        <c:crossAx val="419622272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7108,11 +7108,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376716048"/>
-        <c:axId val="376716440"/>
+        <c:axId val="419623448"/>
+        <c:axId val="419623840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376716048"/>
+        <c:axId val="419623448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7154,7 +7154,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376716440"/>
+        <c:crossAx val="419623840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7162,7 +7162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376716440"/>
+        <c:axId val="419623840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7213,7 +7213,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376716048"/>
+        <c:crossAx val="419623448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7462,11 +7462,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376717224"/>
-        <c:axId val="376717616"/>
+        <c:axId val="419624624"/>
+        <c:axId val="419625016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376717224"/>
+        <c:axId val="419624624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7508,7 +7508,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376717616"/>
+        <c:crossAx val="419625016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7516,7 +7516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376717616"/>
+        <c:axId val="419625016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7567,7 +7567,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376717224"/>
+        <c:crossAx val="419624624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7816,11 +7816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376718400"/>
-        <c:axId val="376718792"/>
+        <c:axId val="419625800"/>
+        <c:axId val="419626192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376718400"/>
+        <c:axId val="419625800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7862,7 +7862,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376718792"/>
+        <c:crossAx val="419626192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7870,7 +7870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376718792"/>
+        <c:axId val="419626192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7921,7 +7921,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376718400"/>
+        <c:crossAx val="419625800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8170,11 +8170,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397069488"/>
-        <c:axId val="397069880"/>
+        <c:axId val="416594408"/>
+        <c:axId val="416594800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397069488"/>
+        <c:axId val="416594408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8216,7 +8216,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397069880"/>
+        <c:crossAx val="416594800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8224,7 +8224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397069880"/>
+        <c:axId val="416594800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8275,7 +8275,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397069488"/>
+        <c:crossAx val="416594408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8524,11 +8524,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397070664"/>
-        <c:axId val="397071056"/>
+        <c:axId val="416595584"/>
+        <c:axId val="416595976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397070664"/>
+        <c:axId val="416595584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8570,7 +8570,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397071056"/>
+        <c:crossAx val="416595976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8578,7 +8578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397071056"/>
+        <c:axId val="416595976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8629,7 +8629,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397070664"/>
+        <c:crossAx val="416595584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8878,11 +8878,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375943176"/>
-        <c:axId val="375976848"/>
+        <c:axId val="435308624"/>
+        <c:axId val="435309016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375943176"/>
+        <c:axId val="435308624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8924,7 +8924,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375976848"/>
+        <c:crossAx val="435309016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8932,7 +8932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375976848"/>
+        <c:axId val="435309016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8983,7 +8983,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375943176"/>
+        <c:crossAx val="435308624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9232,11 +9232,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397071840"/>
-        <c:axId val="397072232"/>
+        <c:axId val="416596760"/>
+        <c:axId val="416597152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397071840"/>
+        <c:axId val="416596760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9278,7 +9278,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397072232"/>
+        <c:crossAx val="416597152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9286,7 +9286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397072232"/>
+        <c:axId val="416597152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9337,7 +9337,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397071840"/>
+        <c:crossAx val="416596760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9586,11 +9586,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397073016"/>
-        <c:axId val="397073408"/>
+        <c:axId val="416597936"/>
+        <c:axId val="416598328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397073016"/>
+        <c:axId val="416597936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9632,7 +9632,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397073408"/>
+        <c:crossAx val="416598328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9640,7 +9640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397073408"/>
+        <c:axId val="416598328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9691,7 +9691,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397073016"/>
+        <c:crossAx val="416597936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9940,11 +9940,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397074192"/>
-        <c:axId val="397074584"/>
+        <c:axId val="416599112"/>
+        <c:axId val="416599504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397074192"/>
+        <c:axId val="416599112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9986,7 +9986,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397074584"/>
+        <c:crossAx val="416599504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9994,7 +9994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397074584"/>
+        <c:axId val="416599504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10045,7 +10045,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397074192"/>
+        <c:crossAx val="416599112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10150,11 +10150,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$8</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>高知餐厅</c:v>
+                  <c:v>川菜</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10185,96 +10185,96 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$8:$AE$8</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$9:$AE$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>456</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1257</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3681</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10690</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11859</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8904</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5905</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3827</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2453</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>472</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2966</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1205</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -10294,11 +10294,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397075368"/>
-        <c:axId val="397075760"/>
+        <c:axId val="416601464"/>
+        <c:axId val="419610552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397075368"/>
+        <c:axId val="416601464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10340,7 +10340,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397075760"/>
+        <c:crossAx val="419610552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10348,7 +10348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397075760"/>
+        <c:axId val="419610552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10399,7 +10399,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397075368"/>
+        <c:crossAx val="416601464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10504,11 +10504,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$9</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>川菜</c:v>
+                  <c:v>一餐清真</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10539,99 +10539,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$9:$AE$9</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$13:$AE$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>456</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>325</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1421</c:v>
+                  <c:v>747</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1257</c:v>
+                  <c:v>2316</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2065</c:v>
+                  <c:v>1409</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3681</c:v>
+                  <c:v>5060</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8370</c:v>
+                  <c:v>11048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10690</c:v>
+                  <c:v>10980</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11859</c:v>
+                  <c:v>4363</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8904</c:v>
+                  <c:v>3017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5905</c:v>
+                  <c:v>2652</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3827</c:v>
+                  <c:v>1393</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2453</c:v>
+                  <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1501</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>973</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>505</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>338</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>141</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>64</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10648,11 +10648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397076544"/>
-        <c:axId val="397118248"/>
+        <c:axId val="419611336"/>
+        <c:axId val="419611728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397076544"/>
+        <c:axId val="419611336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10694,7 +10694,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397118248"/>
+        <c:crossAx val="419611728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10702,7 +10702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397118248"/>
+        <c:axId val="419611728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10753,7 +10753,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397076544"/>
+        <c:crossAx val="419611336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10858,11 +10858,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$13</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>一餐清真</c:v>
+                  <c:v>哈乐之家</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10893,99 +10893,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$13:$AE$13</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$15:$AE$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>430</c:v>
+                  <c:v>5880</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>586</c:v>
+                  <c:v>2165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>747</c:v>
+                  <c:v>1299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2316</c:v>
+                  <c:v>1651</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1409</c:v>
+                  <c:v>1598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5060</c:v>
+                  <c:v>2548</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11048</c:v>
+                  <c:v>7378</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10980</c:v>
+                  <c:v>19107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4363</c:v>
+                  <c:v>32446</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3017</c:v>
+                  <c:v>22416</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2652</c:v>
+                  <c:v>17680</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1393</c:v>
+                  <c:v>10670</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>486</c:v>
+                  <c:v>9190</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>197</c:v>
+                  <c:v>7442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>153</c:v>
+                  <c:v>2951</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>57</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26</c:v>
+                  <c:v>655</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>428</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14</c:v>
+                  <c:v>363</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11002,11 +11002,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397119032"/>
-        <c:axId val="397119424"/>
+        <c:axId val="419612512"/>
+        <c:axId val="419612904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397119032"/>
+        <c:axId val="419612512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11048,7 +11048,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397119424"/>
+        <c:crossAx val="419612904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11056,7 +11056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397119424"/>
+        <c:axId val="419612904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11107,7 +11107,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397119032"/>
+        <c:crossAx val="419612512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11212,11 +11212,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$15</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>哈乐之家</c:v>
+                  <c:v>上海快餐</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11247,99 +11247,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$15:$AE$15</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$16:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>5880</c:v>
+                  <c:v>3273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2165</c:v>
+                  <c:v>3010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1299</c:v>
+                  <c:v>2970</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1651</c:v>
+                  <c:v>6780</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1598</c:v>
+                  <c:v>15867</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2548</c:v>
+                  <c:v>44695</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7378</c:v>
+                  <c:v>59552</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19107</c:v>
+                  <c:v>48468</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32446</c:v>
+                  <c:v>37119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22416</c:v>
+                  <c:v>17124</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17680</c:v>
+                  <c:v>10104</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10670</c:v>
+                  <c:v>5010</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9190</c:v>
+                  <c:v>1960</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7442</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2951</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1323</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>655</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>428</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>363</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>218</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>243</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>131</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>115</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>91</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>70</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>64</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>47</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>29</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>36</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11356,11 +11356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397120208"/>
-        <c:axId val="397120600"/>
+        <c:axId val="419613688"/>
+        <c:axId val="419614080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397120208"/>
+        <c:axId val="419613688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11402,7 +11402,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397120600"/>
+        <c:crossAx val="419614080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11410,7 +11410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397120600"/>
+        <c:axId val="419614080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11461,7 +11461,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397120208"/>
+        <c:crossAx val="419613688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11566,11 +11566,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$16</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>上海快餐</c:v>
+                  <c:v>江南小吃</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11601,99 +11601,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$16:$AE$16</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$18:$AE$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>3273</c:v>
+                  <c:v>1262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3010</c:v>
+                  <c:v>5382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2970</c:v>
+                  <c:v>16644</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6780</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15867</c:v>
+                  <c:v>3185</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44695</c:v>
+                  <c:v>10826</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59552</c:v>
+                  <c:v>13850</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48468</c:v>
+                  <c:v>13300</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37119</c:v>
+                  <c:v>6891</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17124</c:v>
+                  <c:v>11189</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10104</c:v>
+                  <c:v>3455</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5010</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1960</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>490</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>248</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>169</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>81</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11710,11 +11710,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397121384"/>
-        <c:axId val="397121776"/>
+        <c:axId val="419614864"/>
+        <c:axId val="419615256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397121384"/>
+        <c:axId val="419614864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11756,7 +11756,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397121776"/>
+        <c:crossAx val="419615256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11764,7 +11764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397121776"/>
+        <c:axId val="419615256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11815,7 +11815,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397121384"/>
+        <c:crossAx val="419614864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11920,11 +11920,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$18</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>江南小吃</c:v>
+                  <c:v>川味点心</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11955,99 +11955,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$18:$AE$18</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$19:$AE$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1262</c:v>
+                  <c:v>2978</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5382</c:v>
+                  <c:v>22298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16644</c:v>
+                  <c:v>24697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2350</c:v>
+                  <c:v>9959</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3185</c:v>
+                  <c:v>15255</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10826</c:v>
+                  <c:v>15248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13850</c:v>
+                  <c:v>22266</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13300</c:v>
+                  <c:v>13233</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6891</c:v>
+                  <c:v>7071</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11189</c:v>
+                  <c:v>4219</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3455</c:v>
+                  <c:v>6481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>286</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>212</c:v>
+                  <c:v>901</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>170</c:v>
+                  <c:v>4623</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55</c:v>
+                  <c:v>18245</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>61</c:v>
+                  <c:v>3006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>56</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12064,11 +12064,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397122560"/>
-        <c:axId val="397122952"/>
+        <c:axId val="419616040"/>
+        <c:axId val="419616432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397122560"/>
+        <c:axId val="419616040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12110,7 +12110,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397122952"/>
+        <c:crossAx val="419616432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12118,7 +12118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397122952"/>
+        <c:axId val="419616432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12169,7 +12169,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397122560"/>
+        <c:crossAx val="419616040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12274,11 +12274,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$19</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>川味点心</c:v>
+                  <c:v>大众餐厅</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12309,99 +12309,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$19:$AE$19</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$20:$AE$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2978</c:v>
+                  <c:v>2606</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22298</c:v>
+                  <c:v>2462</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24697</c:v>
+                  <c:v>3771</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9959</c:v>
+                  <c:v>2033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15255</c:v>
+                  <c:v>5223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15248</c:v>
+                  <c:v>15893</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22266</c:v>
+                  <c:v>48368</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13233</c:v>
+                  <c:v>35556</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7071</c:v>
+                  <c:v>32919</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4219</c:v>
+                  <c:v>31957</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6481</c:v>
+                  <c:v>13093</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>460</c:v>
+                  <c:v>6063</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>901</c:v>
+                  <c:v>2352</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>334</c:v>
+                  <c:v>647</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4623</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18245</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3006</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>151</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>586</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>71</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>23</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12418,11 +12418,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397123736"/>
-        <c:axId val="397124128"/>
+        <c:axId val="419617216"/>
+        <c:axId val="419617608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397123736"/>
+        <c:axId val="419617216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12464,7 +12464,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397124128"/>
+        <c:crossAx val="419617608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12472,7 +12472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397124128"/>
+        <c:axId val="419617608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12523,7 +12523,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397123736"/>
+        <c:crossAx val="419617216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12772,11 +12772,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373414816"/>
-        <c:axId val="375623440"/>
+        <c:axId val="435309800"/>
+        <c:axId val="435310192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373414816"/>
+        <c:axId val="435309800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12818,7 +12818,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375623440"/>
+        <c:crossAx val="435310192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12826,7 +12826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375623440"/>
+        <c:axId val="435310192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12877,7 +12877,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373414816"/>
+        <c:crossAx val="435309800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12982,11 +12982,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$20</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>大众餐厅</c:v>
+                  <c:v>二大楼教工餐厅</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13017,99 +13017,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$20:$AE$20</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$22:$AE$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2606</c:v>
+                  <c:v>553</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2462</c:v>
+                  <c:v>1067</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3771</c:v>
+                  <c:v>2528</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2033</c:v>
+                  <c:v>1293</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5223</c:v>
+                  <c:v>1091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15893</c:v>
+                  <c:v>2971</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48368</c:v>
+                  <c:v>5501</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35556</c:v>
+                  <c:v>10553</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32919</c:v>
+                  <c:v>15873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31957</c:v>
+                  <c:v>18275</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13093</c:v>
+                  <c:v>20013</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6063</c:v>
+                  <c:v>13694</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2352</c:v>
+                  <c:v>8033</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>647</c:v>
+                  <c:v>4678</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>230</c:v>
+                  <c:v>2648</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>115</c:v>
+                  <c:v>1677</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40</c:v>
+                  <c:v>880</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="29">
                   <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13126,11 +13126,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397124912"/>
-        <c:axId val="397125304"/>
+        <c:axId val="423141312"/>
+        <c:axId val="423141704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397124912"/>
+        <c:axId val="423141312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13172,7 +13172,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397125304"/>
+        <c:crossAx val="423141704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13180,7 +13180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397125304"/>
+        <c:axId val="423141704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13231,7 +13231,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397124912"/>
+        <c:crossAx val="423141312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13336,11 +13336,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>spend_amount_per_perchase_lunch!$A$22</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>二大楼教工餐厅</c:v>
+                  <c:v>高知餐厅</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13371,99 +13371,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>spend_amount_per_perchase_lunch!$B$22:$AE$22</c:f>
+              <c:f>spend_amount_per_perchase_lunch!$B$8:$AE$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>553</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1067</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2528</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1293</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1091</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2971</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5501</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10553</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15873</c:v>
+                  <c:v>2966</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18275</c:v>
+                  <c:v>1205</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20013</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13694</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8033</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4678</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2648</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1677</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>880</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>603</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>425</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>317</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>281</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>209</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>162</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>84</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>68</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13480,11 +13480,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="397823848"/>
-        <c:axId val="397824240"/>
+        <c:axId val="431124632"/>
+        <c:axId val="431119144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="397823848"/>
+        <c:axId val="431124632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13526,7 +13526,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397824240"/>
+        <c:crossAx val="431119144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13534,7 +13534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397824240"/>
+        <c:axId val="431119144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13585,7 +13585,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397823848"/>
+        <c:crossAx val="431124632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13834,11 +13834,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375624224"/>
-        <c:axId val="375624616"/>
+        <c:axId val="435311368"/>
+        <c:axId val="435311760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375624224"/>
+        <c:axId val="435311368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13880,7 +13880,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375624616"/>
+        <c:crossAx val="435311760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13888,7 +13888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375624616"/>
+        <c:axId val="435311760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13939,7 +13939,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375624224"/>
+        <c:crossAx val="435311368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14188,11 +14188,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375625792"/>
-        <c:axId val="375626184"/>
+        <c:axId val="435312544"/>
+        <c:axId val="435312936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375625792"/>
+        <c:axId val="435312544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14234,7 +14234,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375626184"/>
+        <c:crossAx val="435312936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14242,7 +14242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375626184"/>
+        <c:axId val="435312936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14293,7 +14293,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375625792"/>
+        <c:crossAx val="435312544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14542,11 +14542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375626968"/>
-        <c:axId val="375627360"/>
+        <c:axId val="435313720"/>
+        <c:axId val="435289888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375626968"/>
+        <c:axId val="435313720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14588,7 +14588,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375627360"/>
+        <c:crossAx val="435289888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14596,7 +14596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375627360"/>
+        <c:axId val="435289888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14647,7 +14647,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375626968"/>
+        <c:crossAx val="435313720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14896,11 +14896,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375628144"/>
-        <c:axId val="375628536"/>
+        <c:axId val="435290672"/>
+        <c:axId val="435291064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375628144"/>
+        <c:axId val="435290672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14942,7 +14942,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375628536"/>
+        <c:crossAx val="435291064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14950,7 +14950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375628536"/>
+        <c:axId val="435291064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15001,7 +15001,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375628144"/>
+        <c:crossAx val="435290672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15346,11 +15346,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375629320"/>
-        <c:axId val="375629712"/>
+        <c:axId val="435291848"/>
+        <c:axId val="435292240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375629320"/>
+        <c:axId val="435291848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15393,7 +15393,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375629712"/>
+        <c:crossAx val="435292240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15401,7 +15401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375629712"/>
+        <c:axId val="435292240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15452,7 +15452,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375629320"/>
+        <c:crossAx val="435291848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -38228,15 +38228,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38803,38 +38803,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>623888</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="24" name="图表 23"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -38859,7 +38827,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -38891,7 +38859,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -38923,7 +38891,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -38931,16 +38899,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>528638</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>519113</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38955,7 +38923,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -38987,7 +38955,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -39019,7 +38987,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -39051,7 +39019,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -39073,6 +39041,38 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="32" name="图表 31"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="33" name="图表 32"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -39357,8 +39357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -46404,8 +46404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>